<commit_message>
Mapas de Eficiencia Terminal
</commit_message>
<xml_diff>
--- a/Resource/data/Mapeo de indicadores.xlsx
+++ b/Resource/data/Mapeo de indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seggtogob-my.sharepoint.com/personal/wa_moreno_seg_guanajuato_gob_mx/Documents/Proyectos/Proyectos_de_software/Mapas_estadisticos_2022/Resource/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_99C146FC619C63ED0B74B24C1567FA572F40749D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42213F90-0678-4256-86EA-354FCD3A9D35}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_99C146FC619C63ED0B74B24C1567FA572F40749D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08F90AEF-69B3-4C63-A16F-B1E4CA214218}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cobertura 21-22" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,27 @@
     <sheet name="Eficiencia Terminal 20-21" sheetId="4" r:id="rId4"/>
     <sheet name="Absorción 21-22" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="74">
   <si>
     <t>Preescolar</t>
   </si>
@@ -206,6 +216,51 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Sections/4</t>
+  </si>
+  <si>
+    <t>Thresh1</t>
+  </si>
+  <si>
+    <t>Trhesh11</t>
+  </si>
+  <si>
+    <t>Thresh2</t>
+  </si>
+  <si>
+    <t>Thresh22</t>
+  </si>
+  <si>
+    <t>Thresh3</t>
+  </si>
+  <si>
+    <t>Thresh33</t>
+  </si>
+  <si>
+    <t>Thresh4</t>
+  </si>
+  <si>
+    <t>Thresh44</t>
+  </si>
+  <si>
+    <t>PRIMARIA</t>
+  </si>
+  <si>
+    <t>SECUNDARIA</t>
+  </si>
+  <si>
+    <t>MEDIA SUPERIOR</t>
   </si>
 </sst>
 </file>
@@ -281,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -301,6 +356,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3081,13 +3145,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -3108,13 +3176,13 @@
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="8">
         <v>97.37302537399647</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="8">
         <v>91.212076837989628</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="8">
         <v>64.124801731121892</v>
       </c>
     </row>
@@ -3122,13 +3190,13 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>97.5148568341437</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>87.890137328339577</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>62.063732928679798</v>
       </c>
     </row>
@@ -3136,13 +3204,13 @@
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="9">
         <v>94.466019417475735</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>89.805013927576596</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>64.799094510469729</v>
       </c>
     </row>
@@ -3150,13 +3218,13 @@
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <v>99.009628610729024</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>90.017513134851143</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <v>55.954974582425564</v>
       </c>
     </row>
@@ -3164,13 +3232,13 @@
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <v>98.522167487684726</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>91.721854304635755</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>120.88546679499518</v>
       </c>
     </row>
@@ -3178,13 +3246,13 @@
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <v>103.23222277473893</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>92.522380200105317</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>62.0954003407155</v>
       </c>
     </row>
@@ -3192,13 +3260,13 @@
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <v>91.338582677165348</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>98.214285714285708</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>75</v>
       </c>
     </row>
@@ -3206,13 +3274,13 @@
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <v>95.158959537572258</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>93.697569369756934</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="9">
         <v>61.209612096120964</v>
       </c>
     </row>
@@ -3220,13 +3288,13 @@
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="9">
         <v>96.111786148238153</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
         <v>90.630048465266555</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="9">
         <v>52.139037433155082</v>
       </c>
     </row>
@@ -3234,13 +3302,13 @@
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="9">
         <v>97.242543612830616</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
         <v>89.513108614232209</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="9">
         <v>59.162303664921467</v>
       </c>
     </row>
@@ -3248,13 +3316,13 @@
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>94.377510040160644</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>95.582329317269071</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>68.444444444444443</v>
       </c>
     </row>
@@ -3262,13 +3330,13 @@
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="9">
         <v>97.089947089947088</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>94.269972451790636</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <v>62.13176218532405</v>
       </c>
     </row>
@@ -3276,13 +3344,13 @@
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="9">
         <v>99.319727891156461</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="9">
         <v>86.607142857142861</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="9">
         <v>60.941828254847643</v>
       </c>
     </row>
@@ -3290,13 +3358,13 @@
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="9">
         <v>100.96774193548387</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="9">
         <v>94.271685761047465</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="9">
         <v>70.575692963752658</v>
       </c>
     </row>
@@ -3304,13 +3372,13 @@
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="9">
         <v>98.254012954097433</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="9">
         <v>84.686918784872901</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="9">
         <v>65.226171243941835</v>
       </c>
     </row>
@@ -3318,13 +3386,13 @@
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="9">
         <v>99.591391991283032</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="9">
         <v>94.33588218634948</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="9">
         <v>54.28900402993667</v>
       </c>
     </row>
@@ -3332,13 +3400,13 @@
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="9">
         <v>96.453900709219852</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>90.909090909090907</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="9">
         <v>57.971014492753625</v>
       </c>
     </row>
@@ -3346,13 +3414,13 @@
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="9">
         <v>97.259565667011373</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>91.117181612660133</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="9">
         <v>48.764427345368453</v>
       </c>
     </row>
@@ -3360,13 +3428,13 @@
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="9">
         <v>97.916666666666671</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>95.380434782608702</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="9">
         <v>63.028169014084504</v>
       </c>
     </row>
@@ -3374,13 +3442,13 @@
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="9">
         <v>94.375595805529073</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>90.448791714614501</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="9">
         <v>69.491525423728817</v>
       </c>
     </row>
@@ -3388,13 +3456,13 @@
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="9">
         <v>96.353228711088249</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>86.120565519046991</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="9">
         <v>53.555961564487752</v>
       </c>
     </row>
@@ -3402,13 +3470,13 @@
       <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="9">
         <v>98.268839103869652</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>94.624746450304258</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="9">
         <v>53.734671125975474</v>
       </c>
     </row>
@@ -3416,13 +3484,13 @@
       <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="9">
         <v>97.731568998109637</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>81.333333333333329</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="9">
         <v>61.53846153846154</v>
       </c>
     </row>
@@ -3430,13 +3498,13 @@
       <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="9">
         <v>102.19328307059629</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
         <v>85.171102661596962</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="9">
         <v>59.990462565569864</v>
       </c>
     </row>
@@ -3444,13 +3512,13 @@
       <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="9">
         <v>100.34013605442176</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="9">
         <v>92.834890965732086</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="9">
         <v>62.162162162162161</v>
       </c>
     </row>
@@ -3458,13 +3526,13 @@
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="9">
         <v>95.341981132075475</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="9">
         <v>84.149855907780974</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="9">
         <v>233.25867861142217</v>
       </c>
     </row>
@@ -3472,13 +3540,13 @@
       <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="9">
         <v>98.45928099779897</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <v>88.581314878892726</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="9">
         <v>59.191655801825291</v>
       </c>
     </row>
@@ -3486,13 +3554,13 @@
       <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="9">
         <v>98.500778816199372</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="9">
         <v>93.814221126181664</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="9">
         <v>55.920923859855158</v>
       </c>
     </row>
@@ -3500,13 +3568,13 @@
       <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="9">
         <v>97.388059701492537</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="9">
         <v>93.455657492354746</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="9">
         <v>57.637231503579955</v>
       </c>
     </row>
@@ -3514,13 +3582,13 @@
       <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="9">
         <v>99.483204134366929</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="9">
         <v>89.892183288409697</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="9">
         <v>55.050505050505052</v>
       </c>
     </row>
@@ -3528,13 +3596,13 @@
       <c r="A32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="9">
         <v>99.213188460097413</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="9">
         <v>87.537602062741726</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="9">
         <v>40</v>
       </c>
     </row>
@@ -3542,13 +3610,13 @@
       <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="9">
         <v>93.585174625801855</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="9">
         <v>87.08931050439611</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="9">
         <v>50.872210953346858</v>
       </c>
     </row>
@@ -3556,13 +3624,13 @@
       <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="9">
         <v>102.30125523012552</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="9">
         <v>93.876491956408927</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="9">
         <v>59.832134292565947</v>
       </c>
     </row>
@@ -3570,13 +3638,13 @@
       <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="9">
         <v>99.340900768949098</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="9">
         <v>93.243761996161226</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="9">
         <v>55.7713858797161</v>
       </c>
     </row>
@@ -3584,13 +3652,13 @@
       <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="9">
         <v>101.78571428571429</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="9">
         <v>100</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="9">
         <v>52.127659574468083</v>
       </c>
     </row>
@@ -3598,13 +3666,13 @@
       <c r="A37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="9">
         <v>97.127937336814625</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="9">
         <v>90.943877551020407</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="9">
         <v>53.76569037656904</v>
       </c>
     </row>
@@ -3612,13 +3680,13 @@
       <c r="A38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="9">
         <v>96</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="9">
         <v>94.117647058823536</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="9">
         <v>32.142857142857146</v>
       </c>
     </row>
@@ -3626,13 +3694,13 @@
       <c r="A39" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="9">
         <v>96.474358974358978</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="9">
         <v>90.719882468168464</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="9">
         <v>51.116009920088182</v>
       </c>
     </row>
@@ -3640,13 +3708,13 @@
       <c r="A40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="9">
         <v>107.72727272727273</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="9">
         <v>81.742738589211612</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="9">
         <v>70.408163265306129</v>
       </c>
     </row>
@@ -3654,13 +3722,13 @@
       <c r="A41" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="9">
         <v>98.099415204678365</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="9">
         <v>92.229729729729726</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="9">
         <v>50.717703349282296</v>
       </c>
     </row>
@@ -3668,13 +3736,13 @@
       <c r="A42" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="9">
         <v>96.473551637279598</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="9">
         <v>95.180722891566262</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="9">
         <v>62.091503267973856</v>
       </c>
     </row>
@@ -3682,13 +3750,13 @@
       <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="9">
         <v>96.966413867822325</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="9">
         <v>93.548387096774192</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="9">
         <v>67.590361445783131</v>
       </c>
     </row>
@@ -3696,13 +3764,13 @@
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="9">
         <v>97.552447552447546</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="9">
         <v>92.092651757188492</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="9">
         <v>66.93418940609952</v>
       </c>
     </row>
@@ -3710,13 +3778,13 @@
       <c r="A45" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="9">
         <v>100</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="9">
         <v>96.674584323040378</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="9">
         <v>70.606060606060609</v>
       </c>
     </row>
@@ -3724,13 +3792,13 @@
       <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="9">
         <v>101.86234817813765</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="9">
         <v>93.963463065925339</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="9">
         <v>54.554263565891475</v>
       </c>
     </row>
@@ -3738,13 +3806,13 @@
       <c r="A47" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="9">
         <v>102.40963855421687</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="9">
         <v>91.162790697674424</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="9">
         <v>59.25925925925926</v>
       </c>
     </row>
@@ -3752,18 +3820,234 @@
       <c r="A48" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="9">
         <v>94.255319148936167</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="9">
         <v>90.032679738562095</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="9">
         <v>65.73705179282868</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="9">
+        <f>MIN(B3:B48)</f>
+        <v>91.338582677165348</v>
+      </c>
+      <c r="C50" s="9">
+        <f t="shared" ref="C50:D50" si="0">MIN(C3:C48)</f>
+        <v>81.333333333333329</v>
+      </c>
+      <c r="D50" s="9">
+        <f t="shared" si="0"/>
+        <v>32.142857142857146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="9">
+        <f>MAX(B3:B48)</f>
+        <v>107.72727272727273</v>
+      </c>
+      <c r="C51" s="9">
+        <f t="shared" ref="C51:D51" si="1">MAX(C3:C48)</f>
+        <v>100</v>
+      </c>
+      <c r="D51" s="9">
+        <f t="shared" si="1"/>
+        <v>233.25867861142217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="9">
+        <f>B51-B50</f>
+        <v>16.388690050107385</v>
+      </c>
+      <c r="C52" s="9">
+        <f t="shared" ref="C52:D52" si="2">C51-C50</f>
+        <v>18.666666666666671</v>
+      </c>
+      <c r="D52" s="9">
+        <f t="shared" si="2"/>
+        <v>201.11582146856503</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="9">
+        <f>B52/4</f>
+        <v>4.0971725125268463</v>
+      </c>
+      <c r="C53" s="9">
+        <f t="shared" ref="C53:D53" si="3">C52/4</f>
+        <v>4.6666666666666679</v>
+      </c>
+      <c r="D53" s="9">
+        <f t="shared" si="3"/>
+        <v>50.278955367141258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="9">
+        <f>B50</f>
+        <v>91.338582677165348</v>
+      </c>
+      <c r="C54" s="9">
+        <f t="shared" ref="C54:D54" si="4">C50</f>
+        <v>81.333333333333329</v>
+      </c>
+      <c r="D54" s="9">
+        <f t="shared" si="4"/>
+        <v>32.142857142857146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="9">
+        <f>B54+B53</f>
+        <v>95.435755189692202</v>
+      </c>
+      <c r="C55" s="9">
+        <f t="shared" ref="C55:D55" si="5">C54+C53</f>
+        <v>86</v>
+      </c>
+      <c r="D55" s="9">
+        <f t="shared" si="5"/>
+        <v>82.421812509998404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="9">
+        <f>B55+0.01</f>
+        <v>95.445755189692207</v>
+      </c>
+      <c r="C56" s="9">
+        <f t="shared" ref="C56:D56" si="6">C55+0.01</f>
+        <v>86.01</v>
+      </c>
+      <c r="D56" s="9">
+        <f t="shared" si="6"/>
+        <v>82.431812509998409</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="9">
+        <f>B56+B53</f>
+        <v>99.54292770221906</v>
+      </c>
+      <c r="C57" s="9">
+        <f t="shared" ref="C57:D57" si="7">C56+C53</f>
+        <v>90.676666666666677</v>
+      </c>
+      <c r="D57" s="9">
+        <f t="shared" si="7"/>
+        <v>132.71076787713966</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="9">
+        <f>B57+0.01</f>
+        <v>99.552927702219066</v>
+      </c>
+      <c r="C58" s="9">
+        <f t="shared" ref="C58:D58" si="8">C57+0.01</f>
+        <v>90.686666666666682</v>
+      </c>
+      <c r="D58" s="9">
+        <f t="shared" si="8"/>
+        <v>132.72076787713965</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="9">
+        <f>B58+B53</f>
+        <v>103.65010021474592</v>
+      </c>
+      <c r="C59" s="9">
+        <f t="shared" ref="C59:D59" si="9">C58+C53</f>
+        <v>95.353333333333353</v>
+      </c>
+      <c r="D59" s="9">
+        <f t="shared" si="9"/>
+        <v>182.99972324428091</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="9">
+        <f>B59+0.01</f>
+        <v>103.66010021474592</v>
+      </c>
+      <c r="C60" s="9">
+        <f t="shared" ref="C60:D60" si="10">C59+0.01</f>
+        <v>95.363333333333358</v>
+      </c>
+      <c r="D60" s="9">
+        <f t="shared" si="10"/>
+        <v>183.00972324428091</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="9">
+        <f>B51</f>
+        <v>107.72727272727273</v>
+      </c>
+      <c r="C61" s="9">
+        <f t="shared" ref="C61:D61" si="11">C51</f>
+        <v>100</v>
+      </c>
+      <c r="D61" s="9">
+        <f t="shared" si="11"/>
+        <v>233.25867861142217</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3771,7 +4055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4637,18 +4921,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4670,6 +4954,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A74642DA-498C-4A5B-8C8A-E25409904D69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DAE2CF2-CF2B-4A07-862B-44D34329C44F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -4683,12 +4975,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A74642DA-498C-4A5B-8C8A-E25409904D69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
RIMA HSE Primaria y Secundaria
</commit_message>
<xml_diff>
--- a/Resource/data/Mapeo de indicadores.xlsx
+++ b/Resource/data/Mapeo de indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seggtogob-my.sharepoint.com/personal/wa_moreno_seg_guanajuato_gob_mx/Documents/Proyectos/Proyectos_de_software/Mapas_estadisticos_2022/Resource/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_99C146FC619C63ED0B74B24C1567FA572F40749D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08F90AEF-69B3-4C63-A16F-B1E4CA214218}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_99C146FC619C63ED0B74B24C1567FA572F40749D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC352625-068B-493B-BC7C-8EBF7A03FEE4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3148,7 +3148,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4737,6 +4737,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D5E3B4CE0606F46849A4CF64CF2EACB" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4b7e4a3977ed1fb12f498aa9ab783d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="96c9cd64-4e8a-4571-9673-d1c5ae8b9463" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78aa79acd9190b5aabd7b3413b563782" ns3:_="">
     <xsd:import namespace="96c9cd64-4e8a-4571-9673-d1c5ae8b9463"/>
@@ -4920,15 +4929,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4936,6 +4936,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A74642DA-498C-4A5B-8C8A-E25409904D69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7722397A-C00B-4F50-AE59-F04460ECAD3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4949,14 +4957,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A74642DA-498C-4A5B-8C8A-E25409904D69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>